<commit_message>
Integrate some changes by @qgroom
</commit_message>
<xml_diff>
--- a/data/raw/raw_data.xlsx
+++ b/data/raw/raw_data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11730" activeTab="1"/>
   </bookViews>
@@ -24,9 +19,10 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Quentin Groom</author>
+    <author>REYSERHOVE, Lien</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,81 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-is </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Many people will interprete this as the actual location that observations were made.
-Perhaps change this to region
-If you want to make this univeral then perhaps mention the DwC term stateProvince</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-A statement about the presence or absence of a Taxon within the country between the date of first observation  and last date of observation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,104 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Strickly speeking we are using ISO 8601:2004</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Is this vocab comma safe?
-The vocab you link to has subcatagories with commas, slashes and quotes. Perhaps we should create a git hub page with the same vocab, but with simplified reference terms.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E15" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-during the period specified by first and last observation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Quentin Groom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-during the period specified by first and last observation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E19" authorId="0" shapeId="0">
+    <comment ref="E19" authorId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -295,12 +120,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="A21" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>REYSERHOVE, Lien:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Abundance and occurrenceStatus have a great overlap which is confusing if you ask me. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="77">
   <si>
     <t>scientific name</t>
   </si>
@@ -366,9 +215,6 @@
   </si>
   <si>
     <t>The full scientific name of the kingdom in which the taxon is classified.</t>
-  </si>
-  <si>
-    <t>"Animalia", "Fungi", "Plantae"</t>
   </si>
   <si>
     <t>The full scientific name of the phylum or division in which the taxon is classified.</t>
@@ -445,13 +291,7 @@
     <t>"ICBN", "ICZN", "BC"</t>
   </si>
   <si>
-    <t>The specific description of the place.</t>
-  </si>
-  <si>
     <t>"Flanders', "Wallonia", "Belgium"</t>
-  </si>
-  <si>
-    <t>A statement about the presence or absence of a Taxon at a Location. </t>
   </si>
   <si>
     <r>
@@ -489,15 +329,6 @@
     <t>PREFERRED</t>
   </si>
   <si>
-    <t>"Release: Biological control", "Release: hunting", "escape: aquaculture/mariculture"</t>
-  </si>
-  <si>
-    <t>The pathway through which an alien species arrives in the region. Preferred to use the vocabulary suggested by CBD: https://www.cbd.int/doc/meetings/sbstta/sbstta-18/official/sbstta-18-09-add1-en.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The stage in the invasion process a species has reached. We prefer to use the vocubulary suggested by "Blackburn et al. (2011 ) A proposed unified framework for biological invasions. Trends in Ecology and Evolution. 26: 333-339" </t>
-  </si>
-  <si>
     <t>"Casual" OR "established"</t>
   </si>
   <si>
@@ -556,6 +387,85 @@
   </si>
   <si>
     <t>host</t>
+  </si>
+  <si>
+    <t>Must be an ISO 8601:2004 format: yyyy-mm-dd OR yyyy-mm OR yyyy (https://www.iso.org/iso-8601-date-and-time-format.html)</t>
+  </si>
+  <si>
+    <t>The pathway through which an alien species arrives in the region during the period specified by first and last observation. Preferred to use the vocabulary suggested by CBD: https://www.cbd.int/doc/meetings/sbstta/sbstta-18/official/sbstta-18-09-add1-en.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The stage in the invasion process a species has reached during the period specified by first and last observation. We prefer to use the vocubulary suggested by "Blackburn et al. (2011 ) A proposed unified framework for biological invasions. Trends in Ecology and Evolution. 26: 333-339" </t>
+  </si>
+  <si>
+    <t>A statement about the presence or absence of a Taxon within the country between the date of first observation  and last date of observation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The specific description of the place. This applies to a region, a city, a town, etc. This does </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> apply to the actual location that observations were made (so no coordinates) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">YES </t>
+  </si>
+  <si>
+    <t>Is a controlled vocabulary, i.e. one of the seven following kingdoms: "Bacteria", "Archaea", "Protozoa", "Chromista", "Animalia", "Fungi", "Plantae"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">proposed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>controlled vocabulary, see https://github.com/trias-project/vocab/issues/5</t>
+    </r>
+  </si>
+  <si>
+    <t>multiple, separated by semicolon. So each pathway should ideally not include a semicolon</t>
+  </si>
+  <si>
+    <t>multiple, separated by semicolon. So each invasion stage label should ideally not include a semicolon</t>
+  </si>
+  <si>
+    <t>multiple, separated by semicolon. So each habitat label should ideally not include a semicolon</t>
   </si>
 </sst>
 </file>
@@ -620,18 +530,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -726,18 +630,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -753,10 +651,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -772,9 +676,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -812,9 +716,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,7 +753,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -884,7 +788,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1125,7 +1029,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1878,14 +1782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="85.85546875" customWidth="1"/>
     <col min="6" max="6" width="101.28515625" bestFit="1" customWidth="1"/>
@@ -1897,10 +1802,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>36</v>
+        <v>25</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
@@ -1917,13 +1822,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>20</v>
@@ -1937,16 +1842,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
+      <c r="F3" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1957,16 +1862,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1977,16 +1882,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1997,16 +1902,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2017,16 +1922,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2037,16 +1942,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2057,16 +1962,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,16 +1982,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2097,16 +2002,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2114,16 +2019,16 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,16 +2039,16 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2154,16 +2059,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2171,39 +2076,39 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2211,112 +2116,112 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>54</v>
-      </c>
       <c r="F18" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>70</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>65</v>
+      <c r="A22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2334,479 +2239,481 @@
     <col min="1" max="1" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
+    <row r="1" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+        <v>53</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="18"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="16"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="18"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="18"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="16"/>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="16"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="18"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="16"/>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="18"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="18"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="18"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="16"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="18"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="16"/>
     </row>
     <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="18"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="16"/>
     </row>
     <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="18"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="16"/>
     </row>
     <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="18"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="16"/>
     </row>
     <row r="21" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="18"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="16"/>
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="18"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="18"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="18"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="18"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="16"/>
     </row>
     <row r="27" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="18"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B7:O7"/>
-    <mergeCell ref="A1:O2"/>
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B4:O4"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="B6:O6"/>
+    <mergeCell ref="B26:O26"/>
+    <mergeCell ref="B27:O27"/>
+    <mergeCell ref="B20:O20"/>
+    <mergeCell ref="B21:O21"/>
+    <mergeCell ref="B22:O22"/>
+    <mergeCell ref="B23:O23"/>
+    <mergeCell ref="B24:O24"/>
+    <mergeCell ref="B25:O25"/>
     <mergeCell ref="B19:O19"/>
     <mergeCell ref="B8:O8"/>
     <mergeCell ref="B9:O9"/>
@@ -2819,14 +2726,12 @@
     <mergeCell ref="B16:O16"/>
     <mergeCell ref="B17:O17"/>
     <mergeCell ref="B18:O18"/>
-    <mergeCell ref="B26:O26"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B20:O20"/>
-    <mergeCell ref="B21:O21"/>
-    <mergeCell ref="B22:O22"/>
-    <mergeCell ref="B23:O23"/>
-    <mergeCell ref="B24:O24"/>
-    <mergeCell ref="B25:O25"/>
+    <mergeCell ref="B7:O7"/>
+    <mergeCell ref="A1:O2"/>
+    <mergeCell ref="B3:O3"/>
+    <mergeCell ref="B4:O4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="B6:O6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>